<commit_message>
normaliseren en definitieve datadictionary
</commit_message>
<xml_diff>
--- a/Documentatie/Fase 3/Normaliseren.xlsx
+++ b/Documentatie/Fase 3/Normaliseren.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Patrick\Documents\GitHub\WindowsPhoneApp\Documentatie\Fase 2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="12435" windowHeight="5970"/>
   </bookViews>
@@ -205,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -794,9 +789,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -834,9 +829,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -871,7 +866,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -906,7 +901,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1082,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,6 +1086,7 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
veranderingen aan folder structuur en inlog pagina
</commit_message>
<xml_diff>
--- a/Documentatie/Fase 3/Normaliseren.xlsx
+++ b/Documentatie/Fase 3/Normaliseren.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Patrick\Documents\GitHub\WindowsPhoneApp\Documentatie\Fase 3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="12435" windowHeight="5970"/>
   </bookViews>
@@ -63,9 +68,6 @@
     <t>•date</t>
   </si>
   <si>
-    <t>•time</t>
-  </si>
-  <si>
     <t>•description</t>
   </si>
   <si>
@@ -96,9 +98,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -118,6 +117,12 @@
   </si>
   <si>
     <t>Bachmandiagram</t>
+  </si>
+  <si>
+    <t>•duration</t>
+  </si>
+  <si>
+    <t>duration</t>
   </si>
 </sst>
 </file>
@@ -200,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -789,9 +794,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -829,9 +834,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -866,7 +871,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -901,7 +906,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1077,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,27 +1101,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1136,22 +1141,22 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -1161,57 +1166,57 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1221,10 +1226,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>4</v>
@@ -1232,10 +1237,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>2</v>
@@ -1243,44 +1248,44 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1290,34 +1295,34 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1327,35 +1332,35 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="D57" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="G57" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="H57" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>4</v>
@@ -1363,7 +1368,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C71" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>